<commit_message>
- Corrección de la redacción en el primer riesgo.
</commit_message>
<xml_diff>
--- a/Documentacion/UTN BA - Proyecto Final 2014 - G422 - Análisis de riesgos.xlsx
+++ b/Documentacion/UTN BA - Proyecto Final 2014 - G422 - Análisis de riesgos.xlsx
@@ -44,9 +44,6 @@
     <t>Acción</t>
   </si>
   <si>
-    <t>Falta de soporte oficial y documentación sobre la plataforma</t>
-  </si>
-  <si>
     <t>Dificultad de resolución de algún incoveniente surgido con la plataforma en el desarrollo</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Recurrir a herramientas externas de versionado y almacenamiento del código fuente.</t>
+  </si>
+  <si>
+    <t>Falta de soporte oficial y documentación sobre las plataformas utilizadas en el desarrollo</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -710,6 +710,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1008,7 +1011,7 @@
   <dimension ref="A1:I994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1060,26 +1063,26 @@
       <c r="B2" s="5">
         <v>41766</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30.75" customHeight="1">
@@ -1090,25 +1093,25 @@
         <v>41766</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="38.25">
@@ -1119,25 +1122,25 @@
         <v>41766</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="38.25">
@@ -1148,25 +1151,25 @@
         <v>41766</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51">
@@ -1177,25 +1180,25 @@
         <v>41766</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="63.75">
@@ -1206,80 +1209,80 @@
         <v>41766</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="51">
+    </row>
+    <row r="8" spans="1:9" ht="38.25">
       <c r="A8" s="15">
         <v>8</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="E8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="76.5">
+    </row>
+    <row r="9" spans="1:9" ht="63.75">
       <c r="A9" s="18">
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="E9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="I9" s="15"/>
     </row>
@@ -1288,28 +1291,28 @@
         <v>10</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="E10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75">
@@ -5269,131 +5272,131 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="22"/>
       <c r="B2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="22"/>
       <c r="B3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="22"/>
       <c r="B5" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="C6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="C7" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>

</xml_diff>